<commit_message>
North Dakota water rights update.
North Dakota water rights update.
</commit_message>
<xml_diff>
--- a/NorthDakota/WaterAllocation/ND_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/NorthDakota/WaterAllocation/ND_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\NorthDakota\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AA82B2-FAB0-46AD-8E51-D8D403291322}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DDC66B-B0EF-4A52-90A4-974590C6E84D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="296">
   <si>
     <t>Name</t>
   </si>
@@ -915,6 +915,18 @@
   </si>
   <si>
     <t>*Use custom WaDE made ID</t>
+  </si>
+  <si>
+    <t>Reversed order of owner name to be first + last name.</t>
+  </si>
+  <si>
+    <t>OwnerClassificationCV</t>
+  </si>
+  <si>
+    <t>Army (USA)</t>
+  </si>
+  <si>
+    <t>WSWC defined owner tag.</t>
   </si>
 </sst>
 </file>
@@ -1667,7 +1679,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1927,6 +1939,9 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2286,8 +2301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2331,6 +2346,9 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="72" t="s">
         <v>239</v>
+      </c>
+      <c r="B13" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -4582,10 +4600,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5596,7 +5614,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>101</v>
       </c>
@@ -5628,7 +5646,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>98</v>
       </c>
@@ -5660,7 +5678,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="52" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" s="52" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>100</v>
       </c>
@@ -5692,7 +5710,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="52" t="s">
         <v>155</v>
       </c>
@@ -5724,7 +5742,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>82</v>
       </c>
@@ -5756,7 +5774,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="85" t="s">
         <v>289</v>
       </c>
@@ -5782,7 +5800,7 @@
       <c r="I38" s="69"/>
       <c r="J38" s="83"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>90</v>
       </c>
@@ -5814,7 +5832,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>91</v>
       </c>
@@ -5844,7 +5862,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>99</v>
       </c>
@@ -5876,7 +5894,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>96</v>
       </c>
@@ -5908,50 +5926,50 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>89</v>
+        <v>293</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="F43" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="G43" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="D43" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="88"/>
       <c r="H43" s="38" t="s">
         <v>38</v>
       </c>
       <c r="I43" s="67" t="s">
-        <v>38</v>
+        <v>294</v>
       </c>
       <c r="J43" s="63" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E44" s="24" t="s">
         <v>240</v>
@@ -5965,76 +5983,108 @@
       <c r="H44" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="I44" s="18" t="s">
+      <c r="I44" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" s="63" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="F45" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="H45" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="J44" s="64" t="s">
+      <c r="J45" s="64" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="52" t="s">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="52" t="s">
         <v>149</v>
       </c>
-      <c r="B45" s="53" t="s">
+      <c r="B46" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="C45" s="54" t="s">
+      <c r="C46" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="56" t="s">
+      <c r="D46" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="24" t="s">
+      <c r="E46" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="F45" s="34"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="I45" s="65" t="s">
+      <c r="F46" s="34"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="I46" s="65" t="s">
         <v>132</v>
       </c>
-      <c r="J45" s="63" t="s">
+      <c r="J46" s="63" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B47" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E46" s="24" t="s">
+      <c r="D47" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="F46" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="G46" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="H46" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="I46" s="18" t="s">
+      <c r="F47" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="H47" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="I47" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="J46" s="63" t="s">
+      <c r="J47" s="63" t="s">
         <v>211</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:J46">
-    <sortCondition ref="A14:A46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:J47">
+    <sortCondition ref="A14:A47"/>
   </sortState>
   <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>